<commit_message>
migrated to uv from pip
</commit_message>
<xml_diff>
--- a/data/pointsData.xlsx
+++ b/data/pointsData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>email</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Muskan Sharda</t>
+  </si>
+  <si>
+    <t>vishal.maheshab@gmail.com</t>
   </si>
   <si>
     <t>Vishal M</t>
@@ -273,7 +276,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,13 +286,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -347,7 +344,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -664,7 +661,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="40.57642857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="48.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -720,7 +717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -761,7 +758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -802,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -843,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -884,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -925,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -966,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1007,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1048,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1089,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1212,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1376,7 +1373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -1417,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
@@ -1458,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -1499,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
@@ -1540,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>56</v>
       </c>
@@ -1581,12 +1578,12 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>15</v>
@@ -1622,12 +1619,12 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>15</v>
@@ -1663,12 +1660,12 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>15</v>
@@ -1704,12 +1701,12 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>18</v>
@@ -1745,12 +1742,12 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>18</v>
@@ -1786,12 +1783,12 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>35</v>
@@ -1829,10 +1826,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>35</v>
@@ -1870,10 +1867,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>35</v>
@@ -1911,10 +1908,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>35</v>
@@ -1952,10 +1949,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>35</v>
@@ -1993,10 +1990,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>35</v>
@@ -2034,13 +2031,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D34" s="4">
         <v>5</v>
@@ -2075,13 +2072,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D35" s="4">
         <v>5</v>

</xml_diff>